<commit_message>
Rettet feil i excel-fil og analyse av aktivitetsnivå
</commit_message>
<xml_diff>
--- a/Data/Analyser_p.verdi.xlsx
+++ b/Data/Analyser_p.verdi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/Masteroppgave/Gjeldene_analyser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Breili/Documents/HINN/Masteroppgave/1. NY MASTERPROSJEKT/RESULTATER/Masteroppgave/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A832E25-7456-8B49-A5B2-1B5B035CB9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3AD70-331B-FF4E-9183-A0C159B46B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35260" yWindow="1640" windowWidth="28800" windowHeight="17500" xr2:uid="{CFF79CF6-E2E2-AD4F-8873-64FBE2FFBBC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>vat.itt.p</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>es.ppm</t>
+  </si>
+  <si>
+    <t>act.itt.p</t>
+  </si>
+  <si>
+    <t>act.ppm.p</t>
+  </si>
+  <si>
+    <t>act.pp.p</t>
   </si>
 </sst>
 </file>
@@ -489,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B0E86A-64A0-A148-8295-824F29030311}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,6 +760,35 @@
         <v>0.38696000000000003</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="H11">
+        <v>0.64659999999999995</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.67589999999999995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>